<commit_message>
Reformulada banco de login, criado banco de Cargos. Inicio da orientação à objetos no usuarios
</commit_message>
<xml_diff>
--- a/WorkPlan_Desenvolvimento Qualidade.xlsx
+++ b/WorkPlan_Desenvolvimento Qualidade.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rmoliveira\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fillip Pereira\Desktop\Monitoria\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3892C796-DFC9-4024-B53B-8EACDF852D90}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Desenvolvimentos" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Desenvolvimentos!$A$7:$Q$7</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,12 +28,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Marcia Maria Navarro Lopes</author>
   </authors>
   <commentList>
-    <comment ref="B7" authorId="0" shapeId="0">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -46,7 +47,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E7" authorId="0" shapeId="0">
+    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -60,7 +61,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G7" authorId="0" shapeId="0">
+    <comment ref="G7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -74,7 +75,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H7" authorId="0" shapeId="0">
+    <comment ref="H7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -89,7 +90,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I7" authorId="0" shapeId="0">
+    <comment ref="I7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -103,7 +104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L7" authorId="0" shapeId="0">
+    <comment ref="L7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -117,7 +118,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M7" authorId="0" shapeId="0">
+    <comment ref="M7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -131,7 +132,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N7" authorId="0" shapeId="0">
+    <comment ref="N7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -150,7 +151,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="89">
   <si>
     <t>Overall Status</t>
   </si>
@@ -411,12 +412,18 @@
   </si>
   <si>
     <t>Criação de Formulário</t>
+  </si>
+  <si>
+    <t>31/09</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -789,8 +796,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Normal 4" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 4" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="24">
     <dxf>
@@ -1222,15 +1229,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="-0.499984740745262"/>
   </sheetPr>
   <dimension ref="A1:P80"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E70" sqref="E70"/>
+      <pane ySplit="7" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1409,11 +1416,11 @@
       </c>
       <c r="G9" s="35">
         <f>MIN(G10:G29)</f>
-        <v>0</v>
+        <v>43730</v>
       </c>
       <c r="H9" s="35">
         <f>MAX(H10:H29)</f>
-        <v>0</v>
+        <v>43739</v>
       </c>
       <c r="I9" s="36">
         <f>MAX(I10:I29)</f>
@@ -1425,12 +1432,12 @@
       <c r="M9" s="38"/>
       <c r="N9" s="39">
         <f t="shared" ref="N9" ca="1" si="0">H9-TODAY()</f>
-        <v>-43734</v>
+        <v>5</v>
       </c>
       <c r="O9" s="36"/>
       <c r="P9" s="36"/>
     </row>
-    <row r="10" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A10" s="28"/>
       <c r="B10" s="28"/>
       <c r="C10" s="40"/>
@@ -1441,8 +1448,12 @@
       <c r="F10" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
+      <c r="G10" s="43">
+        <v>43735</v>
+      </c>
+      <c r="H10" s="43">
+        <v>43735</v>
+      </c>
       <c r="I10" s="44"/>
       <c r="J10" s="45"/>
       <c r="K10" s="46"/>
@@ -1450,12 +1461,12 @@
       <c r="M10" s="46"/>
       <c r="N10" s="47">
         <f ca="1">H10-TODAY()</f>
-        <v>-43734</v>
+        <v>1</v>
       </c>
       <c r="O10" s="44"/>
       <c r="P10" s="44"/>
     </row>
-    <row r="11" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" s="28"/>
       <c r="B11" s="28"/>
       <c r="C11" s="40"/>
@@ -1466,8 +1477,12 @@
       <c r="F11" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
+      <c r="G11" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="H11" s="43" t="s">
+        <v>87</v>
+      </c>
       <c r="I11" s="44"/>
       <c r="J11" s="45"/>
       <c r="K11" s="46"/>
@@ -1477,7 +1492,7 @@
       <c r="O11" s="44"/>
       <c r="P11" s="44"/>
     </row>
-    <row r="12" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" s="28"/>
       <c r="B12" s="28"/>
       <c r="C12" s="40"/>
@@ -1488,8 +1503,12 @@
       <c r="F12" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="43"/>
-      <c r="H12" s="43"/>
+      <c r="G12" s="43">
+        <v>43738</v>
+      </c>
+      <c r="H12" s="43">
+        <v>43738</v>
+      </c>
       <c r="I12" s="44"/>
       <c r="J12" s="45"/>
       <c r="K12" s="46"/>
@@ -1499,7 +1518,7 @@
       <c r="O12" s="44"/>
       <c r="P12" s="44"/>
     </row>
-    <row r="13" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" s="28"/>
       <c r="B13" s="28"/>
       <c r="C13" s="40"/>
@@ -1510,8 +1529,12 @@
       <c r="F13" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
+      <c r="G13" s="43">
+        <v>43739</v>
+      </c>
+      <c r="H13" s="43">
+        <v>43739</v>
+      </c>
       <c r="I13" s="44"/>
       <c r="J13" s="45"/>
       <c r="K13" s="46"/>
@@ -1521,7 +1544,7 @@
       <c r="O13" s="44"/>
       <c r="P13" s="44"/>
     </row>
-    <row r="14" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14" s="28"/>
       <c r="B14" s="28"/>
       <c r="C14" s="40"/>
@@ -1532,8 +1555,12 @@
       <c r="F14" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
+      <c r="G14" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H14" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I14" s="44"/>
       <c r="J14" s="45"/>
       <c r="K14" s="46"/>
@@ -1543,7 +1570,7 @@
       <c r="O14" s="44"/>
       <c r="P14" s="44"/>
     </row>
-    <row r="15" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15" s="28"/>
       <c r="B15" s="28"/>
       <c r="C15" s="40"/>
@@ -1554,8 +1581,12 @@
       <c r="F15" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="43"/>
-      <c r="H15" s="43"/>
+      <c r="G15" s="43">
+        <v>43739</v>
+      </c>
+      <c r="H15" s="43">
+        <v>43739</v>
+      </c>
       <c r="I15" s="44"/>
       <c r="J15" s="45"/>
       <c r="K15" s="46"/>
@@ -1565,7 +1596,7 @@
       <c r="O15" s="44"/>
       <c r="P15" s="44"/>
     </row>
-    <row r="16" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="28"/>
       <c r="B16" s="28"/>
       <c r="C16" s="40"/>
@@ -1576,8 +1607,12 @@
       <c r="F16" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G16" s="43"/>
-      <c r="H16" s="43"/>
+      <c r="G16" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H16" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I16" s="44"/>
       <c r="J16" s="45"/>
       <c r="K16" s="46"/>
@@ -1587,7 +1622,7 @@
       <c r="O16" s="44"/>
       <c r="P16" s="44"/>
     </row>
-    <row r="17" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="28"/>
       <c r="B17" s="28"/>
       <c r="C17" s="40"/>
@@ -1598,8 +1633,12 @@
       <c r="F17" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G17" s="43"/>
-      <c r="H17" s="43"/>
+      <c r="G17" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H17" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I17" s="44"/>
       <c r="J17" s="45"/>
       <c r="K17" s="46"/>
@@ -1609,7 +1648,7 @@
       <c r="O17" s="44"/>
       <c r="P17" s="44"/>
     </row>
-    <row r="18" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18" s="28"/>
       <c r="B18" s="28"/>
       <c r="C18" s="40"/>
@@ -1620,8 +1659,12 @@
       <c r="F18" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G18" s="43"/>
-      <c r="H18" s="43"/>
+      <c r="G18" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H18" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I18" s="44"/>
       <c r="J18" s="45"/>
       <c r="K18" s="46"/>
@@ -1631,7 +1674,7 @@
       <c r="O18" s="44"/>
       <c r="P18" s="44"/>
     </row>
-    <row r="19" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19" s="28"/>
       <c r="B19" s="28"/>
       <c r="C19" s="40"/>
@@ -1642,8 +1685,12 @@
       <c r="F19" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
+      <c r="G19" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H19" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I19" s="44"/>
       <c r="J19" s="45"/>
       <c r="K19" s="46"/>
@@ -1653,7 +1700,7 @@
       <c r="O19" s="44"/>
       <c r="P19" s="44"/>
     </row>
-    <row r="20" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A20" s="28"/>
       <c r="B20" s="28"/>
       <c r="C20" s="40"/>
@@ -1664,8 +1711,12 @@
       <c r="F20" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G20" s="43"/>
-      <c r="H20" s="43"/>
+      <c r="G20" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H20" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I20" s="44"/>
       <c r="J20" s="45"/>
       <c r="K20" s="46"/>
@@ -1675,7 +1726,7 @@
       <c r="O20" s="44"/>
       <c r="P20" s="44"/>
     </row>
-    <row r="21" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" s="28"/>
       <c r="B21" s="28"/>
       <c r="C21" s="40"/>
@@ -1686,8 +1737,12 @@
       <c r="F21" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G21" s="43"/>
-      <c r="H21" s="43"/>
+      <c r="G21" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H21" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I21" s="44"/>
       <c r="J21" s="45"/>
       <c r="K21" s="46"/>
@@ -1697,7 +1752,7 @@
       <c r="O21" s="44"/>
       <c r="P21" s="44"/>
     </row>
-    <row r="22" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A22" s="28"/>
       <c r="B22" s="28"/>
       <c r="C22" s="40"/>
@@ -1708,8 +1763,12 @@
       <c r="F22" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G22" s="43"/>
-      <c r="H22" s="43"/>
+      <c r="G22" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H22" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I22" s="44"/>
       <c r="J22" s="45"/>
       <c r="K22" s="46"/>
@@ -1719,7 +1778,7 @@
       <c r="O22" s="44"/>
       <c r="P22" s="44"/>
     </row>
-    <row r="23" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A23" s="28"/>
       <c r="B23" s="28"/>
       <c r="C23" s="40"/>
@@ -1730,8 +1789,12 @@
       <c r="F23" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G23" s="43"/>
-      <c r="H23" s="43"/>
+      <c r="G23" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H23" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I23" s="44"/>
       <c r="J23" s="45"/>
       <c r="K23" s="46"/>
@@ -1741,7 +1804,7 @@
       <c r="O23" s="44"/>
       <c r="P23" s="44"/>
     </row>
-    <row r="24" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A24" s="28"/>
       <c r="B24" s="28"/>
       <c r="C24" s="40"/>
@@ -1752,8 +1815,12 @@
       <c r="F24" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G24" s="43"/>
-      <c r="H24" s="43"/>
+      <c r="G24" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H24" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I24" s="44"/>
       <c r="J24" s="45"/>
       <c r="K24" s="46"/>
@@ -1763,7 +1830,7 @@
       <c r="O24" s="44"/>
       <c r="P24" s="44"/>
     </row>
-    <row r="25" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A25" s="28"/>
       <c r="B25" s="28"/>
       <c r="C25" s="40"/>
@@ -1774,8 +1841,12 @@
       <c r="F25" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G25" s="43"/>
-      <c r="H25" s="43"/>
+      <c r="G25" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H25" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I25" s="44"/>
       <c r="J25" s="45"/>
       <c r="K25" s="46"/>
@@ -1785,7 +1856,7 @@
       <c r="O25" s="44"/>
       <c r="P25" s="44"/>
     </row>
-    <row r="26" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A26" s="28"/>
       <c r="B26" s="28"/>
       <c r="C26" s="40"/>
@@ -1796,8 +1867,12 @@
       <c r="F26" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G26" s="43"/>
-      <c r="H26" s="43"/>
+      <c r="G26" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H26" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I26" s="44"/>
       <c r="J26" s="45"/>
       <c r="K26" s="46"/>
@@ -1807,7 +1882,7 @@
       <c r="O26" s="44"/>
       <c r="P26" s="44"/>
     </row>
-    <row r="27" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A27" s="28"/>
       <c r="B27" s="28"/>
       <c r="C27" s="40"/>
@@ -1818,8 +1893,12 @@
       <c r="F27" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G27" s="43"/>
-      <c r="H27" s="43"/>
+      <c r="G27" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H27" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I27" s="44"/>
       <c r="J27" s="45"/>
       <c r="K27" s="46"/>
@@ -1829,7 +1908,7 @@
       <c r="O27" s="44"/>
       <c r="P27" s="44"/>
     </row>
-    <row r="28" spans="1:16" s="21" customFormat="1" ht="15" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="28"/>
       <c r="B28" s="28"/>
       <c r="C28" s="33"/>
@@ -1842,11 +1921,11 @@
       </c>
       <c r="G28" s="35">
         <f>MIN(G29:G35)</f>
-        <v>0</v>
+        <v>43730</v>
       </c>
       <c r="H28" s="35">
         <f>MAX(H29:H35)</f>
-        <v>0</v>
+        <v>43739</v>
       </c>
       <c r="I28" s="36">
         <f>MAX(I29:I37)</f>
@@ -1858,12 +1937,12 @@
       <c r="M28" s="38"/>
       <c r="N28" s="39">
         <f t="shared" ref="N28" ca="1" si="1">H28-TODAY()</f>
-        <v>-43734</v>
+        <v>5</v>
       </c>
       <c r="O28" s="36"/>
       <c r="P28" s="36"/>
     </row>
-    <row r="29" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A29" s="28"/>
       <c r="B29" s="28"/>
       <c r="C29" s="40"/>
@@ -1874,8 +1953,12 @@
       <c r="F29" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G29" s="43"/>
-      <c r="H29" s="43"/>
+      <c r="G29" s="43">
+        <v>43731</v>
+      </c>
+      <c r="H29" s="43">
+        <v>43735</v>
+      </c>
       <c r="I29" s="44"/>
       <c r="J29" s="45">
         <v>3</v>
@@ -1885,12 +1968,12 @@
       <c r="M29" s="46"/>
       <c r="N29" s="47">
         <f ca="1">H29-TODAY()</f>
-        <v>-43734</v>
+        <v>1</v>
       </c>
       <c r="O29" s="44"/>
       <c r="P29" s="44"/>
     </row>
-    <row r="30" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A30" s="28"/>
       <c r="B30" s="28"/>
       <c r="C30" s="40"/>
@@ -1901,8 +1984,12 @@
       <c r="F30" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G30" s="43"/>
-      <c r="H30" s="43"/>
+      <c r="G30" s="43">
+        <v>43730</v>
+      </c>
+      <c r="H30" s="43">
+        <v>43739</v>
+      </c>
       <c r="I30" s="44"/>
       <c r="J30" s="45"/>
       <c r="K30" s="46"/>
@@ -1912,7 +1999,7 @@
       <c r="O30" s="44"/>
       <c r="P30" s="44"/>
     </row>
-    <row r="31" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A31" s="28"/>
       <c r="B31" s="28"/>
       <c r="C31" s="40"/>
@@ -1923,8 +2010,12 @@
       <c r="F31" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G31" s="43"/>
-      <c r="H31" s="43"/>
+      <c r="G31" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H31" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I31" s="44"/>
       <c r="J31" s="45">
         <v>2</v>
@@ -1936,7 +2027,7 @@
       <c r="O31" s="44"/>
       <c r="P31" s="44"/>
     </row>
-    <row r="32" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A32" s="28"/>
       <c r="B32" s="28"/>
       <c r="C32" s="40"/>
@@ -1947,8 +2038,12 @@
       <c r="F32" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G32" s="43"/>
-      <c r="H32" s="43"/>
+      <c r="G32" s="43">
+        <v>43731</v>
+      </c>
+      <c r="H32" s="43">
+        <v>43732</v>
+      </c>
       <c r="I32" s="44"/>
       <c r="J32" s="45">
         <v>1</v>
@@ -1962,7 +2057,7 @@
       <c r="O32" s="44"/>
       <c r="P32" s="44"/>
     </row>
-    <row r="33" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A33" s="28"/>
       <c r="B33" s="28"/>
       <c r="C33" s="40"/>
@@ -1973,8 +2068,12 @@
       <c r="F33" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G33" s="43"/>
-      <c r="H33" s="43"/>
+      <c r="G33" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H33" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I33" s="44"/>
       <c r="J33" s="45"/>
       <c r="K33" s="46"/>
@@ -1984,7 +2083,7 @@
       <c r="O33" s="44"/>
       <c r="P33" s="44"/>
     </row>
-    <row r="34" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C34" s="48"/>
       <c r="D34" s="46"/>
       <c r="E34" s="46" t="s">
@@ -1993,8 +2092,12 @@
       <c r="F34" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="G34" s="43"/>
-      <c r="H34" s="43"/>
+      <c r="G34" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H34" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I34" s="44"/>
       <c r="J34" s="45"/>
       <c r="K34" s="46"/>
@@ -2004,7 +2107,7 @@
       <c r="O34" s="44"/>
       <c r="P34" s="44"/>
     </row>
-    <row r="35" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C35" s="48"/>
       <c r="D35" s="46"/>
       <c r="E35" s="46" t="s">
@@ -2013,8 +2116,12 @@
       <c r="F35" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="G35" s="43"/>
-      <c r="H35" s="43"/>
+      <c r="G35" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H35" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I35" s="44"/>
       <c r="J35" s="45"/>
       <c r="K35" s="46"/>
@@ -2024,7 +2131,7 @@
       <c r="O35" s="44"/>
       <c r="P35" s="44"/>
     </row>
-    <row r="36" spans="1:16" s="21" customFormat="1" ht="15" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="28"/>
       <c r="B36" s="28"/>
       <c r="C36" s="33"/>
@@ -2058,7 +2165,7 @@
       <c r="O36" s="36"/>
       <c r="P36" s="36"/>
     </row>
-    <row r="37" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A37" s="28"/>
       <c r="B37" s="28"/>
       <c r="C37" s="40"/>
@@ -2069,8 +2176,12 @@
       <c r="F37" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G37" s="43"/>
-      <c r="H37" s="43"/>
+      <c r="G37" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H37" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I37" s="44">
         <v>43434</v>
       </c>
@@ -2080,14 +2191,14 @@
       <c r="K37" s="46"/>
       <c r="L37" s="46"/>
       <c r="M37" s="46"/>
-      <c r="N37" s="47">
+      <c r="N37" s="47" t="e">
         <f ca="1">H37-TODAY()</f>
-        <v>-43734</v>
+        <v>#VALUE!</v>
       </c>
       <c r="O37" s="44"/>
       <c r="P37" s="44"/>
     </row>
-    <row r="38" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A38" s="28"/>
       <c r="B38" s="28"/>
       <c r="C38" s="40"/>
@@ -2098,8 +2209,12 @@
       <c r="F38" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G38" s="43"/>
-      <c r="H38" s="43"/>
+      <c r="G38" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H38" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I38" s="44"/>
       <c r="J38" s="45">
         <v>2</v>
@@ -2111,7 +2226,7 @@
       <c r="O38" s="44"/>
       <c r="P38" s="44"/>
     </row>
-    <row r="39" spans="1:16" s="21" customFormat="1" ht="15" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="28"/>
       <c r="B39" s="28"/>
       <c r="C39" s="33"/>
@@ -2145,7 +2260,7 @@
       <c r="O39" s="36"/>
       <c r="P39" s="36"/>
     </row>
-    <row r="40" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A40" s="28"/>
       <c r="B40" s="28"/>
       <c r="C40" s="40"/>
@@ -2156,8 +2271,12 @@
       <c r="F40" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G40" s="43"/>
-      <c r="H40" s="43"/>
+      <c r="G40" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H40" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I40" s="44">
         <v>43434</v>
       </c>
@@ -2167,14 +2286,14 @@
       <c r="K40" s="46"/>
       <c r="L40" s="46"/>
       <c r="M40" s="46"/>
-      <c r="N40" s="47">
+      <c r="N40" s="47" t="e">
         <f ca="1">H40-TODAY()</f>
-        <v>-43734</v>
+        <v>#VALUE!</v>
       </c>
       <c r="O40" s="44"/>
       <c r="P40" s="44"/>
     </row>
-    <row r="41" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A41" s="28"/>
       <c r="B41" s="28"/>
       <c r="C41" s="40"/>
@@ -2185,8 +2304,12 @@
       <c r="F41" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G41" s="43"/>
-      <c r="H41" s="43"/>
+      <c r="G41" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H41" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I41" s="44"/>
       <c r="J41" s="45">
         <v>2</v>
@@ -2198,7 +2321,7 @@
       <c r="O41" s="44"/>
       <c r="P41" s="44"/>
     </row>
-    <row r="42" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A42" s="28"/>
       <c r="B42" s="28"/>
       <c r="C42" s="40"/>
@@ -2209,8 +2332,12 @@
       <c r="F42" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G42" s="43"/>
-      <c r="H42" s="43"/>
+      <c r="G42" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H42" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I42" s="44"/>
       <c r="J42" s="45">
         <v>1</v>
@@ -2224,7 +2351,7 @@
       <c r="O42" s="44"/>
       <c r="P42" s="44"/>
     </row>
-    <row r="43" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A43" s="28"/>
       <c r="B43" s="28"/>
       <c r="C43" s="40"/>
@@ -2235,8 +2362,12 @@
       <c r="F43" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G43" s="43"/>
-      <c r="H43" s="43"/>
+      <c r="G43" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H43" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I43" s="44"/>
       <c r="J43" s="45"/>
       <c r="K43" s="46"/>
@@ -2246,7 +2377,7 @@
       <c r="O43" s="44"/>
       <c r="P43" s="44"/>
     </row>
-    <row r="44" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C44" s="48"/>
       <c r="D44" s="46"/>
       <c r="E44" s="46" t="s">
@@ -2255,8 +2386,12 @@
       <c r="F44" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="G44" s="43"/>
-      <c r="H44" s="43"/>
+      <c r="G44" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H44" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I44" s="44"/>
       <c r="J44" s="45"/>
       <c r="K44" s="46"/>
@@ -2266,7 +2401,7 @@
       <c r="O44" s="44"/>
       <c r="P44" s="44"/>
     </row>
-    <row r="45" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C45" s="48"/>
       <c r="D45" s="46"/>
       <c r="E45" s="46" t="s">
@@ -2275,8 +2410,12 @@
       <c r="F45" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="G45" s="43"/>
-      <c r="H45" s="43"/>
+      <c r="G45" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H45" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I45" s="44"/>
       <c r="J45" s="45"/>
       <c r="K45" s="46"/>
@@ -2286,7 +2425,7 @@
       <c r="O45" s="44"/>
       <c r="P45" s="44"/>
     </row>
-    <row r="46" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C46" s="49"/>
       <c r="D46" s="46"/>
       <c r="E46" s="46" t="s">
@@ -2295,8 +2434,12 @@
       <c r="F46" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="G46" s="43"/>
-      <c r="H46" s="43"/>
+      <c r="G46" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H46" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I46" s="44"/>
       <c r="J46" s="45"/>
       <c r="K46" s="46"/>
@@ -2306,7 +2449,7 @@
       <c r="O46" s="44"/>
       <c r="P46" s="44"/>
     </row>
-    <row r="47" spans="1:16" s="21" customFormat="1" ht="15" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="28"/>
       <c r="B47" s="28"/>
       <c r="C47" s="33"/>
@@ -2318,12 +2461,12 @@
         <v>28</v>
       </c>
       <c r="G47" s="35">
-        <f ca="1">MIN(G48:G54)</f>
-        <v>43734</v>
+        <f>MIN(G48:G54)</f>
+        <v>0</v>
       </c>
       <c r="H47" s="35">
-        <f ca="1">MAX(H48:H54)</f>
-        <v>43734</v>
+        <f>MAX(H48:H54)</f>
+        <v>0</v>
       </c>
       <c r="I47" s="36">
         <f>MAX(I48:I56)</f>
@@ -2335,12 +2478,12 @@
       <c r="M47" s="38"/>
       <c r="N47" s="39">
         <f t="shared" ref="N47" ca="1" si="4">H47-TODAY()</f>
-        <v>0</v>
+        <v>-43734</v>
       </c>
       <c r="O47" s="36"/>
       <c r="P47" s="36"/>
     </row>
-    <row r="48" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A48" s="28"/>
       <c r="B48" s="28"/>
       <c r="C48" s="40"/>
@@ -2351,13 +2494,11 @@
       <c r="F48" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G48" s="43">
-        <f ca="1">TODAY()</f>
-        <v>43734</v>
-      </c>
-      <c r="H48" s="43">
-        <f ca="1">TODAY()</f>
-        <v>43734</v>
+      <c r="G48" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H48" s="43" t="s">
+        <v>88</v>
       </c>
       <c r="I48" s="44">
         <v>43434</v>
@@ -2368,14 +2509,14 @@
       <c r="K48" s="46"/>
       <c r="L48" s="46"/>
       <c r="M48" s="46"/>
-      <c r="N48" s="47">
+      <c r="N48" s="47" t="e">
         <f ca="1">H48-TODAY()</f>
-        <v>0</v>
+        <v>#VALUE!</v>
       </c>
       <c r="O48" s="44"/>
       <c r="P48" s="44"/>
     </row>
-    <row r="49" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A49" s="28"/>
       <c r="B49" s="28"/>
       <c r="C49" s="40"/>
@@ -2386,8 +2527,12 @@
       <c r="F49" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G49" s="43"/>
-      <c r="H49" s="43"/>
+      <c r="G49" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H49" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I49" s="44"/>
       <c r="J49" s="45">
         <v>2</v>
@@ -2399,7 +2544,7 @@
       <c r="O49" s="44"/>
       <c r="P49" s="44"/>
     </row>
-    <row r="50" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A50" s="28"/>
       <c r="B50" s="28"/>
       <c r="C50" s="40"/>
@@ -2410,8 +2555,12 @@
       <c r="F50" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G50" s="43"/>
-      <c r="H50" s="43"/>
+      <c r="G50" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H50" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I50" s="44"/>
       <c r="J50" s="45">
         <v>1</v>
@@ -2425,7 +2574,7 @@
       <c r="O50" s="44"/>
       <c r="P50" s="44"/>
     </row>
-    <row r="51" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A51" s="28"/>
       <c r="B51" s="28"/>
       <c r="C51" s="40"/>
@@ -2436,8 +2585,12 @@
       <c r="F51" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G51" s="43"/>
-      <c r="H51" s="43"/>
+      <c r="G51" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H51" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I51" s="44"/>
       <c r="J51" s="45"/>
       <c r="K51" s="46"/>
@@ -2447,7 +2600,7 @@
       <c r="O51" s="44"/>
       <c r="P51" s="44"/>
     </row>
-    <row r="52" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C52" s="48"/>
       <c r="D52" s="46"/>
       <c r="E52" s="46" t="s">
@@ -2456,8 +2609,12 @@
       <c r="F52" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="G52" s="43"/>
-      <c r="H52" s="43"/>
+      <c r="G52" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H52" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I52" s="44"/>
       <c r="J52" s="45"/>
       <c r="K52" s="46"/>
@@ -2467,7 +2624,7 @@
       <c r="O52" s="44"/>
       <c r="P52" s="44"/>
     </row>
-    <row r="53" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C53" s="48"/>
       <c r="D53" s="46"/>
       <c r="E53" s="46" t="s">
@@ -2476,8 +2633,12 @@
       <c r="F53" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="G53" s="43"/>
-      <c r="H53" s="43"/>
+      <c r="G53" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H53" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I53" s="44"/>
       <c r="J53" s="45"/>
       <c r="K53" s="46"/>
@@ -2487,7 +2648,7 @@
       <c r="O53" s="44"/>
       <c r="P53" s="44"/>
     </row>
-    <row r="54" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C54" s="49"/>
       <c r="D54" s="46"/>
       <c r="E54" s="46" t="s">
@@ -2496,8 +2657,12 @@
       <c r="F54" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="G54" s="43"/>
-      <c r="H54" s="43"/>
+      <c r="G54" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H54" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I54" s="44"/>
       <c r="J54" s="45"/>
       <c r="K54" s="46"/>
@@ -2507,7 +2672,7 @@
       <c r="O54" s="44"/>
       <c r="P54" s="44"/>
     </row>
-    <row r="55" spans="1:16" s="21" customFormat="1" ht="15" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="28"/>
       <c r="B55" s="28"/>
       <c r="C55" s="33"/>
@@ -2519,12 +2684,12 @@
         <v>28</v>
       </c>
       <c r="G55" s="35">
-        <f ca="1">MIN(G56:G60)</f>
-        <v>43734</v>
+        <f>MIN(G56:G60)</f>
+        <v>0</v>
       </c>
       <c r="H55" s="35">
-        <f ca="1">MAX(H56:H60)</f>
-        <v>43734</v>
+        <f>MAX(H56:H60)</f>
+        <v>0</v>
       </c>
       <c r="I55" s="36">
         <f>MAX(I56:I62)</f>
@@ -2536,12 +2701,12 @@
       <c r="M55" s="38"/>
       <c r="N55" s="39">
         <f t="shared" ref="N55" ca="1" si="5">H55-TODAY()</f>
-        <v>0</v>
+        <v>-43734</v>
       </c>
       <c r="O55" s="36"/>
       <c r="P55" s="36"/>
     </row>
-    <row r="56" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A56" s="28"/>
       <c r="B56" s="28"/>
       <c r="C56" s="40"/>
@@ -2552,13 +2717,11 @@
       <c r="F56" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G56" s="43">
-        <f ca="1">TODAY()</f>
-        <v>43734</v>
-      </c>
-      <c r="H56" s="43">
-        <f ca="1">TODAY()</f>
-        <v>43734</v>
+      <c r="G56" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H56" s="43" t="s">
+        <v>88</v>
       </c>
       <c r="I56" s="44">
         <v>43434</v>
@@ -2569,14 +2732,14 @@
       <c r="K56" s="46"/>
       <c r="L56" s="46"/>
       <c r="M56" s="46"/>
-      <c r="N56" s="47">
+      <c r="N56" s="47" t="e">
         <f ca="1">H56-TODAY()</f>
-        <v>0</v>
+        <v>#VALUE!</v>
       </c>
       <c r="O56" s="44"/>
       <c r="P56" s="44"/>
     </row>
-    <row r="57" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A57" s="28"/>
       <c r="B57" s="28"/>
       <c r="C57" s="40"/>
@@ -2587,8 +2750,12 @@
       <c r="F57" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G57" s="43"/>
-      <c r="H57" s="43"/>
+      <c r="G57" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H57" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I57" s="44"/>
       <c r="J57" s="45">
         <v>2</v>
@@ -2600,7 +2767,7 @@
       <c r="O57" s="44"/>
       <c r="P57" s="44"/>
     </row>
-    <row r="58" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A58" s="28"/>
       <c r="B58" s="28"/>
       <c r="C58" s="40"/>
@@ -2611,8 +2778,12 @@
       <c r="F58" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G58" s="43"/>
-      <c r="H58" s="43"/>
+      <c r="G58" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H58" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I58" s="44"/>
       <c r="J58" s="45">
         <v>1</v>
@@ -2626,7 +2797,7 @@
       <c r="O58" s="44"/>
       <c r="P58" s="44"/>
     </row>
-    <row r="59" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A59" s="28"/>
       <c r="B59" s="28"/>
       <c r="C59" s="40"/>
@@ -2637,8 +2808,12 @@
       <c r="F59" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G59" s="43"/>
-      <c r="H59" s="43"/>
+      <c r="G59" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H59" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I59" s="44"/>
       <c r="J59" s="45"/>
       <c r="K59" s="46"/>
@@ -2648,7 +2823,7 @@
       <c r="O59" s="44"/>
       <c r="P59" s="44"/>
     </row>
-    <row r="60" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C60" s="48"/>
       <c r="D60" s="46"/>
       <c r="E60" s="46" t="s">
@@ -2657,8 +2832,12 @@
       <c r="F60" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="G60" s="43"/>
-      <c r="H60" s="43"/>
+      <c r="G60" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H60" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I60" s="44"/>
       <c r="J60" s="45"/>
       <c r="K60" s="46"/>
@@ -2668,7 +2847,7 @@
       <c r="O60" s="44"/>
       <c r="P60" s="44"/>
     </row>
-    <row r="61" spans="1:16" s="21" customFormat="1" ht="15" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="28"/>
       <c r="B61" s="28"/>
       <c r="C61" s="33"/>
@@ -2680,12 +2859,12 @@
         <v>28</v>
       </c>
       <c r="G61" s="35">
-        <f ca="1">MIN(G62:G65)</f>
-        <v>43734</v>
+        <f>MIN(G62:G65)</f>
+        <v>0</v>
       </c>
       <c r="H61" s="35">
-        <f ca="1">MAX(H62:H65)</f>
-        <v>43734</v>
+        <f>MAX(H62:H65)</f>
+        <v>0</v>
       </c>
       <c r="I61" s="36">
         <f>MAX(I62:I67)</f>
@@ -2697,12 +2876,12 @@
       <c r="M61" s="38"/>
       <c r="N61" s="39">
         <f t="shared" ref="N61" ca="1" si="6">H61-TODAY()</f>
-        <v>0</v>
+        <v>-43734</v>
       </c>
       <c r="O61" s="36"/>
       <c r="P61" s="36"/>
     </row>
-    <row r="62" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A62" s="28"/>
       <c r="B62" s="28"/>
       <c r="C62" s="40"/>
@@ -2713,13 +2892,11 @@
       <c r="F62" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G62" s="43">
-        <f ca="1">TODAY()</f>
-        <v>43734</v>
-      </c>
-      <c r="H62" s="43">
-        <f ca="1">TODAY()</f>
-        <v>43734</v>
+      <c r="G62" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H62" s="43" t="s">
+        <v>88</v>
       </c>
       <c r="I62" s="44">
         <v>43434</v>
@@ -2730,14 +2907,14 @@
       <c r="K62" s="46"/>
       <c r="L62" s="46"/>
       <c r="M62" s="46"/>
-      <c r="N62" s="47">
+      <c r="N62" s="47" t="e">
         <f ca="1">H62-TODAY()</f>
-        <v>0</v>
+        <v>#VALUE!</v>
       </c>
       <c r="O62" s="44"/>
       <c r="P62" s="44"/>
     </row>
-    <row r="63" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A63" s="28"/>
       <c r="B63" s="28"/>
       <c r="C63" s="40"/>
@@ -2748,8 +2925,12 @@
       <c r="F63" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G63" s="43"/>
-      <c r="H63" s="43"/>
+      <c r="G63" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H63" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I63" s="44"/>
       <c r="J63" s="45">
         <v>2</v>
@@ -2761,7 +2942,7 @@
       <c r="O63" s="44"/>
       <c r="P63" s="44"/>
     </row>
-    <row r="64" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A64" s="28"/>
       <c r="B64" s="28"/>
       <c r="C64" s="40"/>
@@ -2772,8 +2953,12 @@
       <c r="F64" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G64" s="43"/>
-      <c r="H64" s="43"/>
+      <c r="G64" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H64" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I64" s="44"/>
       <c r="J64" s="45">
         <v>1</v>
@@ -2787,7 +2972,7 @@
       <c r="O64" s="44"/>
       <c r="P64" s="44"/>
     </row>
-    <row r="65" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A65" s="28"/>
       <c r="B65" s="28"/>
       <c r="C65" s="40"/>
@@ -2798,8 +2983,12 @@
       <c r="F65" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G65" s="43"/>
-      <c r="H65" s="43"/>
+      <c r="G65" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H65" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I65" s="44"/>
       <c r="J65" s="45"/>
       <c r="K65" s="46"/>
@@ -2809,7 +2998,7 @@
       <c r="O65" s="44"/>
       <c r="P65" s="44"/>
     </row>
-    <row r="66" spans="1:16" s="21" customFormat="1" ht="15" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="28"/>
       <c r="B66" s="28"/>
       <c r="C66" s="33"/>
@@ -2843,7 +3032,7 @@
       <c r="O66" s="36"/>
       <c r="P66" s="36"/>
     </row>
-    <row r="67" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A67" s="28"/>
       <c r="B67" s="28"/>
       <c r="C67" s="40"/>
@@ -2854,8 +3043,12 @@
       <c r="F67" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G67" s="43"/>
-      <c r="H67" s="43"/>
+      <c r="G67" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H67" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I67" s="44">
         <v>43434</v>
       </c>
@@ -2865,14 +3058,14 @@
       <c r="K67" s="46"/>
       <c r="L67" s="46"/>
       <c r="M67" s="46"/>
-      <c r="N67" s="47">
+      <c r="N67" s="47" t="e">
         <f ca="1">H67-TODAY()</f>
-        <v>-43734</v>
+        <v>#VALUE!</v>
       </c>
       <c r="O67" s="44"/>
       <c r="P67" s="44"/>
     </row>
-    <row r="68" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A68" s="28"/>
       <c r="B68" s="28"/>
       <c r="C68" s="40"/>
@@ -2883,8 +3076,12 @@
       <c r="F68" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G68" s="43"/>
-      <c r="H68" s="43"/>
+      <c r="G68" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H68" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I68" s="44"/>
       <c r="J68" s="45">
         <v>2</v>
@@ -2896,7 +3093,7 @@
       <c r="O68" s="44"/>
       <c r="P68" s="44"/>
     </row>
-    <row r="69" spans="1:16" s="21" customFormat="1" ht="15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" s="21" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A69" s="28"/>
       <c r="B69" s="28"/>
       <c r="C69" s="40"/>
@@ -2907,8 +3104,12 @@
       <c r="F69" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G69" s="43"/>
-      <c r="H69" s="43"/>
+      <c r="G69" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H69" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="I69" s="44"/>
       <c r="J69" s="45">
         <v>1</v>
@@ -2922,7 +3123,7 @@
       <c r="O69" s="44"/>
       <c r="P69" s="44"/>
     </row>
-    <row r="70" spans="1:16" s="21" customFormat="1" ht="15" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="28"/>
       <c r="B70" s="28"/>
       <c r="C70" s="33"/>
@@ -3159,7 +3360,7 @@
     </row>
     <row r="80" spans="1:16" collapsed="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <autoFilter ref="A7:Q7"/>
+  <autoFilter ref="A7:Q7" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="N6">
     <cfRule type="cellIs" dxfId="23" priority="65" operator="greaterThanOrEqual">
       <formula>0</formula>

</xml_diff>